<commit_message>
some changes to wording of poorly-formatted requirements
</commit_message>
<xml_diff>
--- a/docs/productbacklog_additional.xlsx
+++ b/docs/productbacklog_additional.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 2" sheetId="1" state="visible" r:id="rId2"/>
@@ -190,13 +190,13 @@
     <t xml:space="preserve">New Backlog Items:</t>
   </si>
   <si>
-    <t xml:space="preserve">As a user, I want to the app to show me the nearest vending machine location at the push of a button, so that I can avoid excessive travel when I am hungry/thirsty.</t>
+    <t xml:space="preserve">As a user, I want the app to show me the nearest vending machine location at the push of a button, so that I can avoid excessive travel when I am hungry/thirsty.</t>
   </si>
   <si>
     <t xml:space="preserve">← Arpit’s idea</t>
   </si>
   <si>
-    <t xml:space="preserve">As a user, I want to the app to show me shortest paths which include bus routes, so that I can reach very far destinations quickly.</t>
+    <t xml:space="preserve">As a user, I want the app to show me shortest paths which include bus routes, so that I can reach very far destinations on campus quickly.</t>
   </si>
   <si>
     <t xml:space="preserve">← from presentation feedback</t>
@@ -520,8 +520,8 @@
   </sheetPr>
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -995,7 +995,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="24.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>22</v>
       </c>

</xml_diff>